<commit_message>
[FIX] Document template + Base
</commit_message>
<xml_diff>
--- a/admin/questions_files/historic/Questions_Base.xlsx
+++ b/admin/questions_files/historic/Questions_Base.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08F9D60-C16E-4970-83B0-F415CF2C9CC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+    <workbookView xWindow="57480" yWindow="-6915" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Questions" sheetId="1" r:id="rId1"/>
-    <sheet name="Textes" sheetId="2" r:id="rId2"/>
-    <sheet name="Introduction" sheetId="3" r:id="rId3"/>
+    <sheet name="Parametres" sheetId="5" r:id="rId1"/>
+    <sheet name="Questions Debut" sheetId="1" r:id="rId2"/>
+    <sheet name="Questions Fin" sheetId="2" r:id="rId3"/>
+    <sheet name="Textes" sheetId="3" r:id="rId4"/>
+    <sheet name="Introduction" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>Intitulé de la question (ex : quelle est votre adresse mail ?)</t>
   </si>
@@ -33,99 +36,102 @@
     <t>Avez-vous utilisé une application de rencontres dans le passé ou utilisez-vous actuellement une application de rencontres ?</t>
   </si>
   <si>
+    <t>LongRadio</t>
+  </si>
+  <si>
+    <t>Oui, j'en ai utilisé par le passé mais je n'en utilise plus</t>
+  </si>
+  <si>
+    <t>Oui, j'utilise actuellement des applications de rencontres</t>
+  </si>
+  <si>
+    <t>Non, je n'ai jamais utilisé d'applications de rencontres</t>
+  </si>
+  <si>
+    <t>Quelles applications de rencontres avez-vous déjà utilisé ou utilisez-vous actuellement ?</t>
+  </si>
+  <si>
+    <t>checkbox, text</t>
+  </si>
+  <si>
+    <t>2, D, E</t>
+  </si>
+  <si>
+    <t>Adopteunmec</t>
+  </si>
+  <si>
+    <t>Meetic</t>
+  </si>
+  <si>
+    <t>Meetic affinity (affiny)</t>
+  </si>
+  <si>
+    <t>Planetromeo</t>
+  </si>
+  <si>
+    <t>Badoo</t>
+  </si>
+  <si>
+    <t>Bumble</t>
+  </si>
+  <si>
+    <t>Happn</t>
+  </si>
+  <si>
+    <t>Hinge</t>
+  </si>
+  <si>
+    <t>Once</t>
+  </si>
+  <si>
+    <t>Tinder</t>
+  </si>
+  <si>
+    <t>PURE</t>
+  </si>
+  <si>
+    <t>Grindr</t>
+  </si>
+  <si>
+    <t>Her</t>
+  </si>
+  <si>
+    <t>Passions - Meet over 50</t>
+  </si>
+  <si>
+    <t>AdultFriendFinder AFF</t>
+  </si>
+  <si>
+    <t>Tomorrow</t>
+  </si>
+  <si>
+    <t>Lovoo</t>
+  </si>
+  <si>
+    <t>Parship</t>
+  </si>
+  <si>
+    <t>Casuallounge</t>
+  </si>
+  <si>
+    <t>Scruff</t>
+  </si>
+  <si>
+    <t>Unitedmen</t>
+  </si>
+  <si>
+    <t>Quand était votre première inscription à un application de rencontres ? (format MM/AAAA)</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Avec quelle frequence utilisiez ou utilisez-vous des applications de rencontres ?</t>
+  </si>
+  <si>
     <t>radio</t>
   </si>
   <si>
-    <t>Oui, j'en ai utilisé par le passé mais je n'en utilise plus</t>
-  </si>
-  <si>
-    <t>Oui, j'utilise actuellement des applications de rencontres</t>
-  </si>
-  <si>
-    <t>Non, je n'ai jamais utilisé d'applications de rencontres</t>
-  </si>
-  <si>
-    <t>Quelles applications de rencontres avez-vous déjà utilisé ou utilisez-vous actuellement ?</t>
-  </si>
-  <si>
-    <t>checkbox, text</t>
-  </si>
-  <si>
-    <t>2, D, E</t>
-  </si>
-  <si>
-    <t>Adopteunmec</t>
-  </si>
-  <si>
-    <t>Meetic</t>
-  </si>
-  <si>
-    <t>Meetic affinity (affiny)</t>
-  </si>
-  <si>
-    <t>Planetromeo</t>
-  </si>
-  <si>
-    <t>Badoo</t>
-  </si>
-  <si>
-    <t>Bumble</t>
-  </si>
-  <si>
-    <t>Happn</t>
-  </si>
-  <si>
-    <t>Hinge</t>
-  </si>
-  <si>
-    <t>Once</t>
-  </si>
-  <si>
-    <t>Tinder</t>
-  </si>
-  <si>
-    <t>PURE</t>
-  </si>
-  <si>
-    <t>Grindr</t>
-  </si>
-  <si>
-    <t>Her</t>
-  </si>
-  <si>
-    <t>Passions - Meet over 50</t>
-  </si>
-  <si>
-    <t>AdultFriendFinder AFF</t>
-  </si>
-  <si>
-    <t>Tomorrow</t>
-  </si>
-  <si>
-    <t>Lovoo</t>
-  </si>
-  <si>
-    <t>Parship</t>
-  </si>
-  <si>
-    <t>Casuallounge</t>
-  </si>
-  <si>
-    <t>Scruff</t>
-  </si>
-  <si>
-    <t>Unitedmen</t>
-  </si>
-  <si>
-    <t>Quand était votre première inscription à un application de rencontres ? (format MM/AAAA)</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Avec quelle frequence utilisiez ou utilisez-vous des applications de rencontres ?</t>
-  </si>
-  <si>
     <t>Plusieurs fois par jour</t>
   </si>
   <si>
@@ -210,37 +216,58 @@
     <t>RGPD</t>
   </si>
   <si>
+    <t xml:space="preserve">Bienvenu.e à l’étude !_x000D_
+Le but de cette étude est de connaître quelles caractéristiques sont importantes pour vous au moment de vous évaluer vous-même et une autre personne de votre attirance._x000D_
+_x000D__x000D_
+Ce questionnaire effectue une récolte de_x000D_
+(1) vos données personnelles : sexe, préférence du sexe recherché, votre expérience sur les applications de rencontres, et dans des relations affectives du passé_x000D_
+(2) des données sur la manière dont vous le remplissez : mouvements de la souris, changements d'avis, ..._x000D_
+(3) des informations de contact si vous souhaitez les renseigner pour donner suite à l’étude_x000D_
+_x000D_
+Ces données seront utilisées à des fins de recherche scientifique à l’École Polytechnique Fédérale de Lausanne en Suisse. L’étude est menée par la chercheuse doctorale Jessica Pidoux._x000D_
+_x000D_
+Vous pouvez à tout moment abandonner la réalisation du questionnaire, faire une demande concernant vos données ou plus de précisions sur l’étude, ainsi que solliciter la suppression de vos données après avoir complété le questionnaire._x000D_
+Pour toute demande envoyez un message à l'adresse mail 'jessica.pidoux@epfl.ch’ </t>
+  </si>
+  <si>
     <t>Validation du RGPD</t>
   </si>
   <si>
+    <t xml:space="preserve">Cochez la case si vous acceptez de participer à cette étude et de donner vos données à des fins de recherche spécifiés ci-dessus. </t>
+  </si>
+  <si>
     <t>Presentation</t>
   </si>
   <si>
-    <t xml:space="preserve">Bienvenu.e à l’étude !
-Le but de cette étude est de connaître quelles caractéristiques sont importantes pour vous au moment de vous évaluer vous-même et une autre personne de votre attirance.
+    <t>Le questionnaire est divisé en trois phases ou tâches que vous devez réaliser : _x000D_
 _x000D_
-Ce questionnaire effectue une récolte de
-(1) vos données personnelles : sexe, préférence du sexe recherché, votre expérience sur les applications de rencontres, et dans des relations affectives du passé
-(2) des données sur la manière dont vous le remplissez : mouvements de la souris, changements d'avis, ...
-(3) des informations de contact si vous souhaitez les renseigner pour donner suite à l’étude
-Ces données seront utilisées à des fins de recherche scientifique à l’École Polytechnique Fédérale de Lausanne en Suisse. L’étude est menée par la chercheuse doctorale Jessica Pidoux.
-Vous pouvez à tout moment abandonner la réalisation du questionnaire, faire une demande concernant vos données ou plus de précisions sur l’étude, ainsi que solliciter la suppression de vos données après avoir complété le questionnaire.
-Pour toute demande envoyez un message à l'adresse mail 'jessica.pidoux@epfl.ch’ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cochez la case si vous acceptez de participer à cette étude et de donner vos données à des fins de recherche spécifiés ci-dessus. </t>
-  </si>
-  <si>
-    <t>Le questionnaire est divisé en trois phases ou tâches que vous devez réaliser : 
-(1) répondre à deux questions de départ
-(2) réaliser un classement des informations qui vous seront présentées. Ici vous devrez déplacer des cartes avec la souris vers une échelle d'importance. Ces cases contiennent des caractéristiques personnelles génériques que vous devez indiquer comme étant importantes ou non pour vous.
+(1) répondre à deux questions de départ_x000D_
+(2) réaliser un classement des informations qui vous seront présentées. Ici vous devrez déplacer des cartes avec la souris vers une échelle d'importance. Ces cases contiennent des caractéristiques personnelles génériques que vous devez indiquer comme étant importantes ou non pour vous._x000D_
 (3) répondre à quelques questions finales. Maximum 7 questions seront posées.</t>
+  </si>
+  <si>
+    <t>Partie paramétré</t>
+  </si>
+  <si>
+    <t>Fragmentation des questions</t>
+  </si>
+  <si>
+    <t>Question Debut</t>
+  </si>
+  <si>
+    <t>Question Fin</t>
+  </si>
+  <si>
+    <t>Combinatoire ( Non fonctionnel pour les questions de début, remplir 0)</t>
+  </si>
+  <si>
+    <t>Type de réponse attendu : "text", "radio" (choix unique), "checkbox" (choix multiple), voir notice pour tout les choix. Si vous souhaitez indiquer un champ "Autre" à votre réponse à choix multiple ou unique, indiquer : "checkbox, text" ou "radio, text"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -272,7 +299,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,6 +395,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -401,6 +447,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -576,30 +639,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3667E4-4B4B-42F2-829A-889E5503089A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="21.34765625" customWidth="1"/>
+    <col min="2" max="2" width="24.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="32.69921875" customWidth="1"/>
+    <col min="2" max="2" width="32.94921875" customWidth="1"/>
+    <col min="3" max="3" width="33.69921875" customWidth="1"/>
+    <col min="4" max="4" width="33.546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="127.8" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.6"/>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.6"/>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.6"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1 D1:X1" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="27.796875" customWidth="1"/>
+    <col min="2" max="2" width="33.25" customWidth="1"/>
+    <col min="3" max="3" width="29.046875" customWidth="1"/>
+    <col min="4" max="4" width="31.69921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:24" ht="118.5" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -619,7 +772,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -693,7 +846,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -704,35 +857,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -741,60 +894,60 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
         <v>51</v>
       </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:24" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -808,95 +961,96 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.6"/>
+  <cols>
+    <col min="1" max="1" width="35.94921875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E4" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="16384" width="11" style="1"/>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:2" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A3" t="s">
         <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A2 A1 A3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>